<commit_message>
Section 49 : Create report chart with store procedure
</commit_message>
<xml_diff>
--- a/TN_Core_Web_App/wwwroot/export-files/Bill_1.xlsx
+++ b/TN_Core_Web_App/wwwroot/export-files/Bill_1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sales Order</t>
   </si>
@@ -60,16 +60,34 @@
     <t>1</t>
   </si>
   <si>
-    <t>product test</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>Product 18</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1,000</t>
+  </si>
+  <si>
+    <t>12,000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>22,000</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Total amount (by word): mười  đồng chẵn</t>
+    <t>34,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total amount (by word): ba mươi bốn nghìn  đồng chẵn</t>
   </si>
   <si>
     <t>11, 10, 2021</t>
@@ -748,22 +766,27 @@
         <v>13</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7">
-        <f ref="E10:E23" t="shared" si="0">C10*D10</f>
-        <v>0</v>
+      <c r="A10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1">
@@ -774,7 +797,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7">
-        <f t="shared" si="0"/>
+        <f ref="E11:E23" t="shared" si="0">C11*D11</f>
         <v>0</v>
       </c>
     </row>
@@ -924,7 +947,7 @@
     </row>
     <row r="24" ht="18" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="5">
@@ -933,12 +956,12 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" ht="30.75" customHeight="1">
       <c r="A26" s="20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -947,18 +970,18 @@
     </row>
     <row r="28">
       <c r="C28" s="23" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
     </row>
     <row r="29">
       <c r="A29" s="24" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="25" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>

</xml_diff>